<commit_message>
Add of two other pages, start of the page that allows to change the themes and subthemes used in the app, home page begining, and links to other pages
</commit_message>
<xml_diff>
--- a/code/wrapper_dash/format_expenses.xlsx
+++ b/code/wrapper_dash/format_expenses.xlsx
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1613754472" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1613754472" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1613754472" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1613754472"/>
+      <pm:revision xmlns:pm="smNativeData" day="1613758627" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1613758627" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1613758627" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1613758627"/>
     </ext>
   </extLst>
 </workbook>
@@ -79,7 +79,7 @@
         <i val="0"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1613754472">
+            <pm:charSpec xmlns:pm="smNativeData" id="1613758627">
               <pm:latin face="Calibri" sz="220" weight="bold" i="0"/>
               <pm:cs/>
               <pm:ea/>
@@ -99,7 +99,7 @@
         <i val="0"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1613754472">
+            <pm:charSpec xmlns:pm="smNativeData" id="1613758627">
               <pm:latin face="Calibri" sz="220" weight="normal" i="0"/>
               <pm:cs/>
               <pm:ea/>
@@ -114,7 +114,8 @@
 - the date must be in format day/month/year
 - there are two possible currencies : euro and canadian dollar. The calculus is done in the app.
 - to except the expenses done during a trip, you can add a trip name in code/data/dates_voyages.json and use this name in the column.
-- the column theme doesn't has to be written all the time : the application detects automatically the name of the company and associate the theme to the company. So if you do your purchases at Wallmart and you enter all the information one time, the next times you will only have to write the price and company name.</t>
+- the column theme doesn't has to be written all the time : the application detects automatically the name of the company and associate the theme to the company. So if you do your purchases at Wallmart and you enter all the information one time, the next times you will only have to write the price and company name.
+- type is used to differenciate payment from card or cash (nothing entered = by card, "liquide" means by cash)</t>
     </r>
   </si>
   <si>
@@ -221,7 +222,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1613754472" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613758627" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -236,7 +237,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1613754472" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613758627" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -252,7 +253,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1613754472" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613758627" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -267,7 +268,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1613754472" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613758627" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -283,7 +284,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1613754472" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613758627" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -344,7 +345,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1613754472" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1613758627" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -366,7 +367,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472"/>
+          <pm:border xmlns:pm="smNativeData" id="1613758627"/>
         </ext>
       </extLst>
     </border>
@@ -385,7 +386,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -406,7 +407,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -428,7 +429,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -449,7 +450,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -470,7 +471,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -491,7 +492,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -513,7 +514,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -535,7 +536,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -558,7 +559,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -580,7 +581,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -603,7 +604,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -625,7 +626,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -647,7 +648,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472">
+          <pm:border xmlns:pm="smNativeData" id="1613758627">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -669,7 +670,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1613754472"/>
+          <pm:border xmlns:pm="smNativeData" id="1613758627"/>
         </ext>
       </extLst>
     </border>
@@ -759,10 +760,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1613754472" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1613758627" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1613754472" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1613758627" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -1044,14 +1045,14 @@
     <col min="9" max="9" width="23.000000" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1613754472" min="9" max="9" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1613758627" min="9" max="9" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
     <col min="10" max="10" width="15.660714" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1613754472" min="10" max="10" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1613758627" min="10" max="10" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
@@ -1059,14 +1060,14 @@
     <col min="13" max="13" width="13.107143" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1613754472" min="13" max="13" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1613758627" min="13" max="13" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
     <col min="14" max="14" width="14.000000" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1613754472" min="14" max="14" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1613758627" min="14" max="14" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
@@ -6111,7 +6112,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1613754472" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1613758627" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -6120,14 +6121,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1613754472" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1613754472" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1613758627" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1613758627" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613754472" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613758627" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -6149,7 +6150,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1613754472" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1613758627" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -6158,14 +6159,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1613754472" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1613754472" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1613758627" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1613758627" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613754472" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613758627" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -6187,7 +6188,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1613754472" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1613758627" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -6196,14 +6197,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1613754472" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1613754472" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1613758627" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1613758627" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613754472" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613758627" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>